<commit_message>
Adding 'PP' tranche to Sale as Tranche 1 with previous tranches 1 - 3 now 2 - 4
</commit_message>
<xml_diff>
--- a/Docs/DAICO Calcs.xlsx
+++ b/Docs/DAICO Calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Pacio\Development\ICO Dapps\DAICO\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA36BD71-930A-429B-919E-3F5767E2115E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0933F2-0D7B-41F3-927D-38DE784B7F8C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25245" windowHeight="11670" xr2:uid="{4168C5EE-3339-4FDC-B848-D7A4D84A183C}"/>
   </bookViews>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
-  <si>
-    <t xml:space="preserve"> Combos</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t xml:space="preserve"> LE_M_FUND_PICOS_MEMBER_B       =   76; // LE_M_FUND_B | LE_PICOS_B | LE_MEMBER_B</t>
   </si>
@@ -41,90 +38,18 @@
     <t xml:space="preserve"> LE_WHITELISTED_MEMBER_B        =   96; // LE_WHITELISTED_B | LE_MEMBER_B</t>
   </si>
   <si>
-    <t xml:space="preserve"> LE_EVER_PRESALE_COMBO_B        =  384; // LE_PRESALE_B | LE_WAS_PRESALE_B</t>
-  </si>
-  <si>
     <t xml:space="preserve"> LE_MEMBER_PROXY_B              = 2112; // LE_MEMBER_B | LE_PROXY_B</t>
   </si>
   <si>
     <t xml:space="preserve"> LE_PROXY_INVOLVED_COMBO_B      = 3072; // LE_PROXY_APPOINTER_B | LE_PROXY_B</t>
   </si>
   <si>
-    <t xml:space="preserve"> LE_BLOCKED_FROM_VOTING_B   =    8192; // 13 Set if a member is blocked from voting by a PGC managed op as a result of trolling etc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_REGISTERED_B            =       1; //  0 Entry has been registered with addedT set but nothing more</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_SALE_CONTRACT_B         =       2; //  1 Is the Sale Contract entry - where the minted PIOs are held. Has dbId == 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_M_FUND_B                =       4; //  2 Mfund funded whitelisted with picos entry or unfunded whitelisted with picos entry. See below for more.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_PICOS_B                 =       8; //  3 Holds Picos. Can be set wo LE_M_FUND_B being set for a presale entry</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_P_FUND_B                =      16; //  4 Pfund prepurchase entry, always funded. There are 4 types of prepurchase entries as below. If unset then entry is an escrow entry, and must then have either LE_WHITELISTED_B or LE_PRESALE_B set or both.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_WHITELISTED_B           =      32; //  5 Has been whitelisted</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_MEMBER_B                =      64; //  6 Is a Pacio Member: Whitelisted with a picosBalance</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_PRESALE_B               =     128; //  7 A Presale List entry - Pacio Seed Presale or Pacio Private Placement - not yet whitelisted</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_WAS_PRESALE_B           =     256; //  8 Was a Presale entry which has been whitelisted</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_FROM_TRANSFER_OK_B      =     512; //  9 Transfers from this entry allowed entry even if pTransfersOkB is false. Is set for the Sale contract entry.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_PROXY_APPOINTER_B       =    1024; // 10 This entry has appointed a Proxy. Need not be a Member.                                              /- one entry can have both bits set</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_PROXY_B                 =    2048; // 11 This entry is a Proxy i.e. one or more other entries have appointed it as a proxy. Must be a Member. |  as a proxy can appoint a proxy</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_DOWNGRADED_B            =    4096; // 12 This entry has been downgraded from whitelisted. Refunding candidate.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_TRANSFERRED_TO_PB_B     =   16384; // 14 This entry has had its PIOs transferred to the Pacio Blockchain</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_P_REFUND_S_CAP_MISS_B   =   32768; // 15 Pfund funds Refund due to soft cap not being reached</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_P_REFUND_SALE_CLOSE_B   =   65536; // 16 Pfund funds Refund due to not being whitelisted by the time that the sale closes</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_P_REFUND_ONCE_OFF_B     =  131072; // 17 Pfund funds Refund once off manually for whatever reason</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_MNP_REFUND_S_CAP_MISS_B =  262144; // 18 Mfund but not presale Refund due to soft cap not being reached</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_M_REFUND_TERMINATION_B  =  524288; // 19 Mfund or Presale with picos Refund proportionately according to Picos held following a vote for project termination</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_M_REFUND_ONCE_OFF_B     = 1048576; // 20 Mfund funds Refunded once off manually for whatever reason including downgrade from whitelisted</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_REFUNDED_COMBO_B         = 2064384; // LE_P_REFUND_S_CAP_MISS_B | LE_P_REFUND_SALE_CLOSE_B | LE_P_REFUND_ONCE_OFF_B | LE_MNP_REFUND_S_CAP_MISS_B | LE_M_REFUND_TERMINATION_B | LE_M_REFUND_ONCE_OFF_B</t>
-  </si>
-  <si>
     <t xml:space="preserve"> LE_DEAD_COMBO_B             = 2080768; // LE_TRANSFERRED_TO_PB_B | LE_REFUNDED_COMBO_B  or bits &gt;= 8192</t>
   </si>
   <si>
     <t xml:space="preserve"> LE_NO_SEND_FUNDS_COMBO_B    = 2084994; // LE_DEAD_COMBO_B | LE_SALE_CONTRACT_B | LE_PRESALE | LE_DOWNGRADED_B</t>
   </si>
   <si>
-    <t xml:space="preserve"> LE_NO_REFUND_COMBO_B        = 2080770; // LE_DEAD_COMBO_B | LE_SALE_CONTRACT_B Starting point check. Could also be more i.e. no funds or no PIOs</t>
-  </si>
-  <si>
     <t xml:space="preserve"> LE_MF_PICOS_MEMBER_PROXY_ALL_B = 3148; // LE_M_FUND_B | LE_PICOS_B | LE_MEMBER_B | LE_PROXY_INVOLVED_COMBO_B</t>
   </si>
   <si>
@@ -132,6 +57,84 @@
   </si>
   <si>
     <t xml:space="preserve"> LE_PROXY_APP_VOTE_BLOCK_B      = 9216; // LE_PROXY_APPOINTER_B | LE_BLOCKED_FROM_VOTING_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_WHITELISTED_P_FUND_B        =   48; // LE_WHITELISTED_B | LE_P_FUND_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_REGISTERED_B                =       1; //  0 Entry has been registered with addedT set but nothing more</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_SALE_CONTRACT_B             =       2; //  1 Is the Sale Contract entry - where the minted PIOs are held. Has dbId == 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_M_FUND_B                    =       4; //  2 Mfund funded whitelisted with picos entry or unfunded whitelisted with picos entry. See below for more.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_PICOS_B                     =       8; //  3 Holds Picos. Can be set wo LE_M_FUND_B being set for a presale entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_P_FUND_B                    =      16; //  4 Pfund prepurchase entry, always funded. There are 4 types of prepurchase entries as below. If unset then entry is an escrow entry, and must then have either LE_WHITELISTED_B or LE_PRESALE_B set or both.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_WHITELISTED_B               =      32; //  5 Has been whitelisted</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_MEMBER_B                    =      64; //  6 Is a Pacio Member: Whitelisted with a picosBalance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_PRESALE_B                   =     128; //  7 A Presale List entry - Pacio Seed Presale or Pacio Private Placement. /- Can make Tranche 1 purchases but not Tranche 2 to 4 ones on same account</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_TRANCH1_B                   =     256; //  8 Was or included a Tranche 1 purchase.                                 |   until after soft cap as not entitled to soft cap miss refund                              -</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_FROM_TRANSFER_OK_B          =     512; //  9 Transfers from this entry allowed entry even if pTransfersOkB is false. Is set for the Sale contract entry.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_PROXY_APPOINTER_B           =    1024; // 10 This entry has appointed a Proxy. Need not be a Member.                                              /- one entry can have both bits set</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_PROXY_B                     =    2048; // 11 This entry is a Proxy i.e. one or more other entries have appointed it as a proxy. Must be a Member. |  as a proxy can appoint a proxy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_DOWNGRADED_B                =    4096; // 12 This entry has been downgraded from whitelisted. Refunding candidate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_BLOCKED_FROM_VOTING_B       =    8192; // 13 Set if a member is blocked from voting by a PGC managed op as a result of trolling etc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_TRANSFERRED_TO_PB_B         =   16384; // 14 This entry has had its PIOs transferred to the Pacio Blockchain</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_P_REFUNDED_S_CAP_MISS_B     =   32768; // 15 Pfund funds Refunded due to soft cap not being reached</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_P_REFUNDED_SALE_CLOSE_B     =   65536; // 16 Pfund funds Refunded due to not being whitelisted by the time that the sale closes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_P_REFUNDED_ONCE_OFF_B       =  131072; // 17 Pfund funds Refunded once off manually for whatever reason</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_M_REFUNDED_S_CAP_MISS_NPT1B =  262144; // 18 Mfund funds Refunded due to soft cap not being reached. Such refunds do not apply to MFunds from a presale or tranche 1 purchase.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_M_REFUNDED_TERMINATION_B    =  524288; // 19 Mfund or Presale with picos Refund proportionately according to Picos held following a vote for project termination</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_M_REFUNDED_ONCE_OFF_B       = 1048576; // 20 Mfund funds Refunded once off manually for whatever reason including downgrade from whitelisted</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> // Combos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_PRESALE_TRANCH1_B           =  384; // LE_PRESALE_B | LE_TRANCH1_B == not eligible for a soft cap miss refund</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_REFUNDED_COMBO_B         = 2064384; // LE_P_REFUNDED_S_CAP_MISS_B | LE_P_REFUNDED_SALE_CLOSE_B | LE_P_REFUNDED_ONCE_OFF_B | LE_M_REFUNDED_S_CAP_MISS_NPT1B | LE_M_REFUNDED_TERMINATION_B | LE_M_REFUNDED_ONCE_OFF_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_NO_REFUNDS_COMBO_B       = 2080770; // LE_DEAD_COMBO_B | LE_SALE_CONTRACT_B Starting point check. Could also be more i.e. no funds or no PIOs</t>
   </si>
 </sst>
 </file>
@@ -491,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575028E4-902E-4BF0-8AA7-825AE5B17B2C}">
-  <dimension ref="A2:C36"/>
+  <dimension ref="A2:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -504,7 +507,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -513,16 +516,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
-        <f t="shared" ref="A4:A23" si="0">A3*2</f>
+        <f t="shared" ref="A4:A13" si="0">A3*2</f>
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -531,7 +534,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -540,7 +543,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -549,7 +552,7 @@
         <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -558,7 +561,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -567,7 +570,7 @@
         <v>128</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -576,7 +579,7 @@
         <v>256</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -585,7 +588,7 @@
         <v>512</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
@@ -594,7 +597,7 @@
         <v>1024</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -603,93 +606,93 @@
         <v>2048</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14">
-        <f>A13*2</f>
+        <f t="shared" ref="A14:A22" si="1">A13*2</f>
         <v>4096</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15">
-        <f>A14*2</f>
+        <f t="shared" si="1"/>
         <v>8192</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16">
-        <f>A15*2</f>
+        <f t="shared" si="1"/>
         <v>16384</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17">
-        <f>A16*2</f>
+        <f t="shared" si="1"/>
         <v>32768</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18">
-        <f>A17*2</f>
+        <f t="shared" si="1"/>
         <v>65536</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19">
-        <f>A18*2</f>
+        <f t="shared" si="1"/>
         <v>131072</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20">
-        <f>A19*2</f>
+        <f t="shared" si="1"/>
         <v>262144</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21">
-        <f>A20*2</f>
+        <f t="shared" si="1"/>
         <v>524288</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22">
-        <f>A21*2</f>
+        <f t="shared" si="1"/>
         <v>1048576</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C23" s="1" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
@@ -698,110 +701,119 @@
         <v>76</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B25">
+        <f>A7+A6</f>
+        <v>48</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B26">
         <f>A7+A8</f>
         <v>96</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B26">
+      <c r="C26" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B27">
         <f>A9+A10</f>
         <v>384</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B27">
+      <c r="C27" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B28">
         <f>A8+A13</f>
         <v>2112</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B28">
+      <c r="C28" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B29">
         <f>A12+A13</f>
         <v>3072</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B29">
+      <c r="C29" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B30">
         <f>A12+A15</f>
         <v>9216</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B30">
+      <c r="C30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B31">
         <f>A4+A5+A8+A12</f>
         <v>1100</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B31">
-        <f>B30+A13</f>
-        <v>3148</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>31</v>
+      <c r="C31" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B32">
+        <f>B31+A13</f>
+        <v>3148</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B33">
         <f>SUM(A17:A22)</f>
         <v>2064384</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B33">
-        <f>B32+A16</f>
-        <v>2080768</v>
-      </c>
       <c r="C33" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B34">
-        <f>B33+A3+A9+A14</f>
-        <v>2084994</v>
+        <f>B33+A16</f>
+        <v>2080768</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B35">
-        <f>B33+A3</f>
+        <f>B34+A3+A9+A14</f>
+        <v>2084994</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B36">
+        <f>B34+A3</f>
         <v>2080770</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="C36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Token Swap ability added
</commit_message>
<xml_diff>
--- a/Docs/DAICO Calcs.xlsx
+++ b/Docs/DAICO Calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Pacio\Development\ICO Dapps\DAICO\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0933F2-0D7B-41F3-927D-38DE784B7F8C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B484D3D5-B4A1-46F3-A361-EE3A07BEAA01}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25245" windowHeight="11670" xr2:uid="{4168C5EE-3339-4FDC-B848-D7A4D84A183C}"/>
   </bookViews>
@@ -30,37 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
-  <si>
-    <t xml:space="preserve"> LE_M_FUND_PICOS_MEMBER_B       =   76; // LE_M_FUND_B | LE_PICOS_B | LE_MEMBER_B</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_WHITELISTED_MEMBER_B        =   96; // LE_WHITELISTED_B | LE_MEMBER_B</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_MEMBER_PROXY_B              = 2112; // LE_MEMBER_B | LE_PROXY_B</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_PROXY_INVOLVED_COMBO_B      = 3072; // LE_PROXY_APPOINTER_B | LE_PROXY_B</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_DEAD_COMBO_B             = 2080768; // LE_TRANSFERRED_TO_PB_B | LE_REFUNDED_COMBO_B  or bits &gt;= 8192</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_NO_SEND_FUNDS_COMBO_B    = 2084994; // LE_DEAD_COMBO_B | LE_SALE_CONTRACT_B | LE_PRESALE | LE_DOWNGRADED_B</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_MF_PICOS_MEMBER_PROXY_ALL_B = 3148; // LE_M_FUND_B | LE_PICOS_B | LE_MEMBER_B | LE_PROXY_INVOLVED_COMBO_B</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_MF_PICOS_MEMBER_PROXY_APP_B = 1100; // LE_M_FUND_B | LE_PICOS_B | LE_MEMBER_B | LE_PROXY_APPOINTER_B</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_PROXY_APP_VOTE_BLOCK_B      = 9216; // LE_PROXY_APPOINTER_B | LE_BLOCKED_FROM_VOTING_B</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_WHITELISTED_P_FUND_B        =   48; // LE_WHITELISTED_B | LE_P_FUND_B</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t xml:space="preserve"> LE_REGISTERED_B                =       1; //  0 Entry has been registered with addedT set but nothing more</t>
   </si>
@@ -68,73 +38,112 @@
     <t xml:space="preserve"> LE_SALE_CONTRACT_B             =       2; //  1 Is the Sale Contract entry - where the minted PIOs are held. Has dbId == 1</t>
   </si>
   <si>
-    <t xml:space="preserve"> LE_M_FUND_B                    =       4; //  2 Mfund funded whitelisted with picos entry or unfunded whitelisted with picos entry. See below for more.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_PICOS_B                     =       8; //  3 Holds Picos. Can be set wo LE_M_FUND_B being set for a presale entry</t>
-  </si>
-  <si>
     <t xml:space="preserve"> LE_P_FUND_B                    =      16; //  4 Pfund prepurchase entry, always funded. There are 4 types of prepurchase entries as below. If unset then entry is an escrow entry, and must then have either LE_WHITELISTED_B or LE_PRESALE_B set or both.</t>
   </si>
   <si>
-    <t xml:space="preserve"> LE_WHITELISTED_B               =      32; //  5 Has been whitelisted</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_MEMBER_B                    =      64; //  6 Is a Pacio Member: Whitelisted with a picosBalance</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_PRESALE_B                   =     128; //  7 A Presale List entry - Pacio Seed Presale or Pacio Private Placement. /- Can make Tranche 1 purchases but not Tranche 2 to 4 ones on same account</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_TRANCH1_B                   =     256; //  8 Was or included a Tranche 1 purchase.                                 |   until after soft cap as not entitled to soft cap miss refund                              -</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_FROM_TRANSFER_OK_B          =     512; //  9 Transfers from this entry allowed entry even if pTransfersOkB is false. Is set for the Sale contract entry.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_PROXY_APPOINTER_B           =    1024; // 10 This entry has appointed a Proxy. Need not be a Member.                                              /- one entry can have both bits set</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_PROXY_B                     =    2048; // 11 This entry is a Proxy i.e. one or more other entries have appointed it as a proxy. Must be a Member. |  as a proxy can appoint a proxy</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_DOWNGRADED_B                =    4096; // 12 This entry has been downgraded from whitelisted. Refunding candidate.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_BLOCKED_FROM_VOTING_B       =    8192; // 13 Set if a member is blocked from voting by a PGC managed op as a result of trolling etc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_TRANSFERRED_TO_PB_B         =   16384; // 14 This entry has had its PIOs transferred to the Pacio Blockchain</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_P_REFUNDED_S_CAP_MISS_B     =   32768; // 15 Pfund funds Refunded due to soft cap not being reached</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_P_REFUNDED_SALE_CLOSE_B     =   65536; // 16 Pfund funds Refunded due to not being whitelisted by the time that the sale closes</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_P_REFUNDED_ONCE_OFF_B       =  131072; // 17 Pfund funds Refunded once off manually for whatever reason</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_M_REFUNDED_S_CAP_MISS_NPT1B =  262144; // 18 Mfund funds Refunded due to soft cap not being reached. Such refunds do not apply to MFunds from a presale or tranche 1 purchase.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_M_REFUNDED_TERMINATION_B    =  524288; // 19 Mfund or Presale with picos Refund proportionately according to Picos held following a vote for project termination</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_M_REFUNDED_ONCE_OFF_B       = 1048576; // 20 Mfund funds Refunded once off manually for whatever reason including downgrade from whitelisted</t>
-  </si>
-  <si>
     <t xml:space="preserve"> // Combos</t>
   </si>
   <si>
-    <t xml:space="preserve"> LE_PRESALE_TRANCH1_B           =  384; // LE_PRESALE_B | LE_TRANCH1_B == not eligible for a soft cap miss refund</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_REFUNDED_COMBO_B         = 2064384; // LE_P_REFUNDED_S_CAP_MISS_B | LE_P_REFUNDED_SALE_CLOSE_B | LE_P_REFUNDED_ONCE_OFF_B | LE_M_REFUNDED_S_CAP_MISS_NPT1B | LE_M_REFUNDED_TERMINATION_B | LE_M_REFUNDED_ONCE_OFF_B</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LE_NO_REFUNDS_COMBO_B       = 2080770; // LE_DEAD_COMBO_B | LE_SALE_CONTRACT_B Starting point check. Could also be more i.e. no funds or no PIOs</t>
+    <t xml:space="preserve"> LE_FUNDED_B                    =       4; //  2 Has contributed wei</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_HOLDS_PICOS_B               =       8; //  3 Holds Picos. Can be set wo LE_CONTRIBUTOR_B being set as the result of a transfer. Can be set wo LE_M_FUND_B being set for a presale entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_M_FUND_B                    =      32; //  5 Mfund funded whitelisted with picos entry or unfunded whitelisted with picos entry. See below for more.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_WHITELISTED_B               =      64; //  6 Has been whitelisted</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_MEMBER_B                    =     128; //  7 Is a Pacio Member: Whitelisted with a picosBalance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_PRESALE_B                   =     256; //  8 A Presale List entry - Pacio Seed Presale or Pacio Private Placement. /- Can make Tranche 1 purchases but not Tranche 2 to 4 ones on same account</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_TRANCH1_B                   =     512; //  9 Was or included a Tranche 1 purchase.                                 |   until after soft cap as not entitled to soft cap miss refund                              -</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_FROM_TRANSFER_OK_B          =    1024; // 10 Transfers from this entry allowed entry even if pTransfersOkB is false. Is set for the Sale contract entry.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_PROXY_APPOINTER_B           =    2048; // 11 This entry has appointed a Proxy. Need not be a Member.                                              /- one entry can have both bits set</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_PROXY_B                     =    4096; // 12 This entry is a Proxy i.e. one or more other entries have appointed it as a proxy. Must be a Member. |  as a proxy can appoint a proxy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_DOWNGRADED_B                =    8192; // 13 This entry has been downgraded from whitelisted. Refunding candidate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_BLOCKED_FROM_VOTING_B       =   16384; // 14 Set if a member is blocked from voting by a PGC managed op as a result of trolling etc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_TRANSFERRED_TO_PB_B         =   32768; // 15 This entry has had its PIOs transferred to the Pacio Blockchain</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_P_REFUNDED_S_CAP_MISS_B     =   65536; // 16 Pfund funds Refunded due to soft cap not being reached</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_P_REFUNDED_SALE_CLOSE_B     =  131072; // 17 Pfund funds Refunded due to not being whitelisted by the time that the sale closes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_P_REFUNDED_ONCE_OFF_B       =  262144; // 18 Pfund funds Refunded once off manually for whatever reason</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_M_REFUNDED_S_CAP_MISS_NPT1B =  524288; // 19 Mfund funds Refunded due to soft cap not being reached. Such refunds do not apply to MFunds from a presale or tranche 1 purchase.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_M_REFUNDED_TERMINATION_B    = 1048576; // 20 Mfund or Presale with picos Refund proportionately according to Picos held following a vote for project termination</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_M_REFUNDED_ONCE_OFF_B       = 2097152; // 21 Mfund funds Refunded once off manually for whatever reason including downgrade from whitelisted</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_FUNDED_P_FUND_B             =      20; // LE_FUNDED_B | LE_P_FUND_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_FUNDED_M_FUND_PICOS_B       =      44; // LE_FUNDED_B | LE_M_FUND_B | LE_HOLDS_PICOS_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_M_FUND_PICOS_MEMBER_B       =     168; // LE_M_FUND_B | LE_HOLDS_PICOS_B | LE_MEMBER_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_WHITELISTED_P_FUND_B        =      80; // LE_WHITELISTED_B | LE_P_FUND_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_WHITELISTED_MEMBER_B        =     192; // LE_WHITELISTED_B | LE_MEMBER_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_PRESALE_TRANCH1_B           =     768; // LE_PRESALE_B | LE_TRANCH1_B == not eligible for a soft cap miss refund</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_MEMBER_PROXY_B              =    4224; // LE_MEMBER_B | LE_PROXY_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_PROXY_INVOLVED_COMBO_B      =    6144; // LE_PROXY_APPOINTER_B | LE_PROXY_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_PROXY_APP_VOTE_BLOCK_B      =   18432; // LE_PROXY_APPOINTER_B | LE_BLOCKED_FROM_VOTING_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_MF_PICOS_MEMBER_PROXY_APP_B =    2216; // LE_M_FUND_B | LE_HOLDS_PICOS_B | LE_MEMBER_B | LE_PROXY_APPOINTER_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_MF_PICOS_MEMBER_PROXY_ALL_B =    6312; // LE_M_FUND_B | LE_HOLDS_PICOS_B | LE_MEMBER_B | LE_PROXY_INVOLVED_COMBO_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_REFUNDED_COMBO_B            = 4128768; // LE_P_REFUNDED_S_CAP_MISS_B | LE_P_REFUNDED_SALE_CLOSE_B | LE_P_REFUNDED_ONCE_OFF_B | LE_M_REFUNDED_S_CAP_MISS_NPT1B | LE_M_REFUNDED_TERMINATION_B | LE_M_REFUNDED_ONCE_OFF_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_DEAD_COMBO_B                = 4161536; // LE_TRANSFERRED_TO_PB_B | LE_REFUNDED_COMBO_B  or bits &gt;= 8192</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_NO_SEND_FUNDS_COMBO_B       = 4169986; // LE_DEAD_COMBO_B | LE_SALE_CONTRACT_B | LE_PRESALE | LE_DOWNGRADED_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_NO_REFUNDS_COMBO_B          = 4161538; // LE_DEAD_COMBO_B | LE_SALE_CONTRACT_B Starting point check. Could also be more i.e. no funds or no PIOs</t>
   </si>
 </sst>
 </file>
@@ -494,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575028E4-902E-4BF0-8AA7-825AE5B17B2C}">
-  <dimension ref="A2:C37"/>
+  <dimension ref="A2:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -507,7 +516,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -516,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -525,7 +534,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -534,7 +543,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -543,7 +552,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -552,7 +561,7 @@
         <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -561,7 +570,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -570,7 +579,7 @@
         <v>128</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -579,7 +588,7 @@
         <v>256</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -588,7 +597,7 @@
         <v>512</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
@@ -597,7 +606,7 @@
         <v>1024</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -606,16 +615,16 @@
         <v>2048</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14">
-        <f t="shared" ref="A14:A22" si="1">A13*2</f>
+        <f t="shared" ref="A14:A23" si="1">A13*2</f>
         <v>4096</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
@@ -624,7 +633,7 @@
         <v>8192</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
@@ -633,7 +642,7 @@
         <v>16384</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
@@ -642,7 +651,7 @@
         <v>32768</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -651,7 +660,7 @@
         <v>65536</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
@@ -660,7 +669,7 @@
         <v>131072</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -669,7 +678,7 @@
         <v>262144</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -678,7 +687,7 @@
         <v>524288</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
@@ -687,133 +696,161 @@
         <v>1048576</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <f t="shared" si="1"/>
+        <v>2097152</v>
+      </c>
       <c r="C23" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B24">
-        <f>A4+A5+A8</f>
-        <v>76</v>
-      </c>
       <c r="C24" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B25">
-        <f>A7+A6</f>
-        <v>48</v>
+        <f>A4+A6</f>
+        <v>20</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B26">
-        <f>A7+A8</f>
-        <v>96</v>
+        <f>A4+A7+A5</f>
+        <v>44</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B27">
-        <f>A9+A10</f>
-        <v>384</v>
+        <f>A5+A7+A9</f>
+        <v>168</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B28">
-        <f>A8+A13</f>
-        <v>2112</v>
+        <f>A6+A8</f>
+        <v>80</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B29">
-        <f>A12+A13</f>
-        <v>3072</v>
+        <f>A8+A9</f>
+        <v>192</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B30">
-        <f>A12+A15</f>
-        <v>9216</v>
+        <f>A10+A11</f>
+        <v>768</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B31">
-        <f>A4+A5+A8+A12</f>
-        <v>1100</v>
+        <f>A9+A14</f>
+        <v>4224</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B32">
-        <f>B31+A13</f>
-        <v>3148</v>
+        <f>A13+A14</f>
+        <v>6144</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B33">
-        <f>SUM(A17:A22)</f>
-        <v>2064384</v>
+        <f>A13+A16</f>
+        <v>18432</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B34">
+        <f>A5+A7+A9+A13</f>
+        <v>2216</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <f>A7+A5+A9+B32</f>
+        <v>6312</v>
+      </c>
+      <c r="B35">
+        <f>B34+A14</f>
+        <v>6312</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B34">
-        <f>B33+A16</f>
-        <v>2080768</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B35">
-        <f>B34+A3+A9+A14</f>
-        <v>2084994</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B36">
-        <f>B34+A3</f>
-        <v>2080770</v>
+        <f>SUM(A18:A23)</f>
+        <v>4128768</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="C37" s="1"/>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B37">
+        <f>B36+A17</f>
+        <v>4161536</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B38">
+        <f>B37+A3+A10+A15</f>
+        <v>4169986</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B39">
+        <f>B37+A3</f>
+        <v>4161538</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change to use offline signing for ManOps 2 New Sale and List contracts wip
</commit_message>
<xml_diff>
--- a/Docs/DAICO Calcs.xlsx
+++ b/Docs/DAICO Calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Pacio\Development\ICO Dapps\DAICO\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9EE86C-5E02-44E7-8E4F-49F007780BEF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A154CF0E-F225-4DC6-B2DC-E2127FBC3C35}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25245" windowHeight="11670" xr2:uid="{4168C5EE-3339-4FDC-B848-D7A4D84A183C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t xml:space="preserve"> LE_REGISTERED_B                =       1; //  0 Entry has been registered with addedT set but nothing more</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t xml:space="preserve"> LE_REFUNDS_NOK_B               = 4161538; // LE_DEAD_B | LE_SALE_CONTRACT_B Starting point check. Could also be more i.e. no funds or no PIOs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LE_SALE_CON_PICOS_FR_TRAN_OK_B =    1034; // LE_SALE_CONTRACT_B | LE_HOLDS_PICOS_B | LE_FROM_TRANSFER_OK_B for the sale contract bit settings</t>
   </si>
 </sst>
 </file>
@@ -578,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575028E4-902E-4BF0-8AA7-825AE5B17B2C}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1045,86 +1048,95 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B54">
+        <f>A25+A27+A34</f>
+        <v>1034</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B55">
         <f>A35+A36</f>
         <v>6144</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B55">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B56">
         <f>A35+A38</f>
         <v>18432</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B56">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B57">
         <f>A27+A29+A31+A35</f>
         <v>2216</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A57">
-        <f>A29+A27+A31+B54</f>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <f>A29+A27+A31+B55</f>
         <v>6312</v>
       </c>
-      <c r="B57">
-        <f>B56+A36</f>
+      <c r="B58">
+        <f>B57+A36</f>
         <v>6312</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B58">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B59">
         <f>SUM(A40:A45)</f>
         <v>4128768</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B59">
-        <f>B58+A39</f>
-        <v>4161536</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B60">
-        <f>B59+A25+A32+A37</f>
-        <v>4169986</v>
+        <f>B59+A39</f>
+        <v>4161536</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B61">
-        <f>B59+A25</f>
-        <v>4161538</v>
+        <f>B60+A25+A32+A37</f>
+        <v>4169986</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B62">
-        <f>B59+A25</f>
+        <f>B60+A25</f>
         <v>4161538</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B63">
+        <f>B60+A25</f>
+        <v>4161538</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>